<commit_message>
reportes excel y otras cosas - by criferlo
</commit_message>
<xml_diff>
--- a/default/app/temp/templates_informes/template_evaluacionproveedores.xlsx
+++ b/default/app/temp/templates_informes/template_evaluacionproveedores.xlsx
@@ -156,6 +156,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,7 +169,6 @@
     <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,7 +520,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,30 +537,30 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -568,11 +568,11 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
@@ -587,11 +587,11 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="9">
+      <c r="D5" s="10">
         <v>40225</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="4">
         <v>1</v>
       </c>
@@ -630,48 +630,48 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>